<commit_message>
Convert excel unicode encoding (_x000D_) into real unicode
</commit_message>
<xml_diff>
--- a/examples/string.xlsx
+++ b/examples/string.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000" calcMode="manual" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>string</t>
   </si>
@@ -31,6 +31,21 @@
   </si>
   <si>
     <t>Result</t>
+  </si>
+  <si>
+    <t>- Fuel combustion efficiency of cars improves by ~19%;
+|- Plug-in hybrids and electric cars efficiency improves by ~30%;
+|- Fuel combustion, hybrid and electric buses efficiency improves by ~15%;
+|- Rail transport efficiency improves by ~10%</t>
+  </si>
+  <si>
+    <t>With line breaks</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Linked</t>
   </si>
 </sst>
 </file>
@@ -66,8 +81,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,13 +420,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -430,6 +455,32 @@
       <c r="B3" t="str">
         <f>B1&amp;B2</f>
         <v>hello world3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="60">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="str">
+        <f>B4&amp;" One"</f>
+        <v>- Fuel combustion efficiency of cars improves by ~19%;_x000D_|- Plug-in hybrids and electric cars efficiency improves by ~30%;_x000D_|- Fuel combustion, hybrid and electric buses efficiency improves by ~15%;_x000D_|- Rail transport efficiency improves by ~10% One</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="str">
+        <f>B4</f>
+        <v>- Fuel combustion efficiency of cars improves by ~19%;_x000D_|- Plug-in hybrids and electric cars efficiency improves by ~30%;_x000D_|- Fuel combustion, hybrid and electric buses efficiency improves by ~15%;_x000D_|- Rail transport efficiency improves by ~10%</v>
       </c>
     </row>
   </sheetData>

</xml_diff>